<commit_message>
Updated BOM and added photos of built module
</commit_message>
<xml_diff>
--- a/PlaitsPartsMU.xlsx
+++ b/PlaitsPartsMU.xlsx
@@ -677,9 +677,6 @@
     <t>Female Pin Header 4 Pin</t>
   </si>
   <si>
-    <t>Male Pin Header 10 pin and 4 pin. Buy a 40 pin and cut to length.</t>
-  </si>
-  <si>
     <t>40 Pin 2.54mm Single Row Pin Header Strip</t>
   </si>
   <si>
@@ -714,6 +711,9 @@
   </si>
   <si>
     <t>963-TMK212ABJ225MD-T</t>
+  </si>
+  <si>
+    <t>Male Pin Header 10 pin and two 4 pin. Buy a 40 pin and cut to length.</t>
   </si>
 </sst>
 </file>
@@ -983,6 +983,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -994,9 +997,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1348,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1368,16 +1368,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1410,20 +1410,20 @@
       <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="9"/>
       <c r="I3" s="42"/>
       <c r="J3" s="41"/>
     </row>
-    <row r="4" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="J4" s="41"/>
     </row>
-    <row r="5" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="J5" s="41"/>
     </row>
-    <row r="6" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="J6" s="41"/>
     </row>
-    <row r="7" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="J7" s="41"/>
     </row>
-    <row r="8" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="J8" s="41"/>
     </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="J9" s="41"/>
     </row>
-    <row r="10" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>27</v>
       </c>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="J10" s="41"/>
     </row>
-    <row r="11" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>30</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="J11" s="41"/>
     </row>
-    <row r="12" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>33</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="J12" s="41"/>
     </row>
-    <row r="13" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="J13" s="41"/>
     </row>
-    <row r="14" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>39</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>60</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>69</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>79</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>83</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>88</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="J26" s="41"/>
     </row>
-    <row r="27" spans="1:10" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>101</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:1025" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1025" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>142</v>
       </c>
@@ -2434,15 +2434,15 @@
       <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:1025" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
       <c r="H38" s="29"/>
       <c r="I38" s="42"/>
       <c r="J38" s="41"/>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="J42" s="41"/>
     </row>
-    <row r="43" spans="1:1025" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1025" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>177</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1025" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>180</v>
       </c>
@@ -3710,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I51" s="42" t="s">
         <v>217</v>
-      </c>
-      <c r="I51" s="42" t="s">
-        <v>218</v>
       </c>
       <c r="J51" s="41" t="s">
         <v>196</v>
@@ -3724,10 +3724,10 @@
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I52" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J52" s="41" t="s">
         <v>196</v>
@@ -3737,11 +3737,11 @@
       <c r="B53" s="1">
         <v>1</v>
       </c>
-      <c r="C53" s="48" t="s">
+      <c r="C53" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="I53" s="42" t="s">
         <v>221</v>
-      </c>
-      <c r="I53" s="42" t="s">
-        <v>222</v>
       </c>
       <c r="J53" s="41" t="s">
         <v>196</v>
@@ -3749,7 +3749,7 @@
     </row>
     <row r="54" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -3773,7 +3773,7 @@
     </row>
     <row r="55" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -3782,14 +3782,14 @@
         <v>48</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F55" s="19" t="str">
         <f>"0805"</f>
         <v>0805</v>
       </c>
       <c r="I55" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J55" s="41" t="s">
         <v>196</v>
@@ -3797,7 +3797,7 @@
     </row>
     <row r="56" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="57" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -3837,7 +3837,7 @@
         <v>0805</v>
       </c>
       <c r="I57" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J57" s="41" t="s">
         <v>195</v>

</xml_diff>